<commit_message>
Finalização CRUD prateleira e documentar Status Report
-
</commit_message>
<xml_diff>
--- a/Documentos do Projeto/Estimativa_Projeto.xlsx
+++ b/Documentos do Projeto/Estimativa_Projeto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SuperMaps\Documentos do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{68682496-DBC1-4CF8-B96C-17FDFBB30A86}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B0E00ACC-83E2-4B70-8A6D-D697FB9EF5C3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="136">
   <si>
     <t>Estimativa de Esforço de Projeto baseado em                                                                Pontos de Caso de Uso (vs 1.1)</t>
   </si>
@@ -587,69 +587,9 @@
     <t>Homens/hora por RFS</t>
   </si>
   <si>
-    <t>Consumidores</t>
-  </si>
-  <si>
     <t>Administrador</t>
   </si>
   <si>
-    <t>[RFS02] Cadastrar Mapa</t>
-  </si>
-  <si>
-    <t>[RFS01] Importar Banco de Dados do Supermercado</t>
-  </si>
-  <si>
-    <t>[RFS03] Editar Mapa</t>
-  </si>
-  <si>
-    <t>[RFS04] Remover Mapa</t>
-  </si>
-  <si>
-    <t>[RFS05] Consultar Mapa</t>
-  </si>
-  <si>
-    <t>[RFS06] Cadastrar Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS07] Editar Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS08] Consultar Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS09] Remover Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS10] Inserir Prateleira no Mapa</t>
-  </si>
-  <si>
-    <t>[RFS11] Inserir Produtos na Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS12] Remover Produto na Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS13] Atualizar Produto na Prateleira</t>
-  </si>
-  <si>
-    <t>[RFS14] Consultar Produto</t>
-  </si>
-  <si>
-    <t>[RFS15] Localizar Produto no Supermercado</t>
-  </si>
-  <si>
-    <t>[RFS16] Calcular menor caminhos para compras</t>
-  </si>
-  <si>
-    <t>[RFS18] Ranking de Produtos</t>
-  </si>
-  <si>
-    <t>[RFS19] Relatório de itens mais visitados no supermercado</t>
-  </si>
-  <si>
-    <t>[RFS17] Emissão do menor caminho</t>
-  </si>
-  <si>
     <t>SuperMaps</t>
   </si>
   <si>
@@ -657,6 +597,81 @@
   </si>
   <si>
     <t>14/05/2018</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>[RF01] Cadastrar Produto</t>
+  </si>
+  <si>
+    <t>[RF02] Cadastrar Usuário</t>
+  </si>
+  <si>
+    <t>[RF03] Consultar Usuário</t>
+  </si>
+  <si>
+    <t>[RF04] Editar Usuário</t>
+  </si>
+  <si>
+    <t>[RF05] Remover Usuário</t>
+  </si>
+  <si>
+    <t>[RF06] Cadastrar Mapa</t>
+  </si>
+  <si>
+    <t>[RF07] Editar Mapa</t>
+  </si>
+  <si>
+    <t>[RF08] Remover Mapa</t>
+  </si>
+  <si>
+    <t>[RF09] Consultar Mapa</t>
+  </si>
+  <si>
+    <t>[RF10] Cadastrar Prateleira</t>
+  </si>
+  <si>
+    <t>[RF11] Editar Prateleira</t>
+  </si>
+  <si>
+    <t>[RF12] Consultar Prateleira</t>
+  </si>
+  <si>
+    <t>[RF13] Remover Prateleira</t>
+  </si>
+  <si>
+    <t>[RF14] Inserir Prateleira no Mapa</t>
+  </si>
+  <si>
+    <t>[RF15] Inserir Produtos na Prateleira</t>
+  </si>
+  <si>
+    <t>[RF16] Remover Produto na Prateleira</t>
+  </si>
+  <si>
+    <t>[RF17] Editar Produto na Prateleira</t>
+  </si>
+  <si>
+    <t>[RF18] Consultar Produto</t>
+  </si>
+  <si>
+    <t>[RF19] Localizar Produto no Supermercado</t>
+  </si>
+  <si>
+    <t>[RF20] Calcular menor caminho para compras</t>
+  </si>
+  <si>
+    <t>[RF21] Emissão do menor caminho</t>
+  </si>
+  <si>
+    <t>[RF22] Ranking de Produtos</t>
+  </si>
+  <si>
+    <t>[RF23] Relatório de itens mais visitados no supermercado</t>
   </si>
 </sst>
 </file>
@@ -1656,49 +1671,13 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1712,6 +1691,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1723,11 +1746,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1735,22 +1761,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2441,7 +2456,7 @@
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2486,32 +2501,32 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
       <c r="K3" s="2"/>
       <c r="L3"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="2"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -2531,54 +2546,54 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="107" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="123" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="109" t="s">
-        <v>129</v>
-      </c>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="124" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="110" t="s">
+      <c r="B8" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="110"/>
+      <c r="C8" s="116"/>
       <c r="D8" s="3" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="108" t="s">
+      <c r="F8" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="108"/>
+      <c r="G8" s="117"/>
       <c r="H8" s="3">
         <v>1</v>
       </c>
@@ -2591,12 +2606,12 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
       <c r="J9" s="6"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -2631,18 +2646,18 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
       <c r="F12"/>
-      <c r="G12" s="113" t="s">
+      <c r="G12" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
       <c r="J12" s="7" t="s">
         <v>7</v>
       </c>
@@ -2653,24 +2668,23 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="114" t="s">
+      <c r="B13" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
       <c r="E13" s="9">
-        <f>Atores!D10+'RFS ou RFC'!D10</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F13"/>
-      <c r="G13" s="114" t="s">
+      <c r="G13" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="114"/>
-      <c r="I13" s="114"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
       <c r="J13" s="10">
         <f t="shared" ref="J13:J20" si="0">$E$13*$E$14*K13</f>
-        <v>12.693333333333333</v>
+        <v>4.2</v>
       </c>
       <c r="K13" s="11">
         <f>dadoshistoricos!E31</f>
@@ -2680,24 +2694,23 @@
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="114" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="115"/>
-      <c r="D14" s="115"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="114"/>
       <c r="E14" s="13">
-        <f>dadoshistoricos!L30</f>
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="F14"/>
-      <c r="G14" s="116" t="s">
+      <c r="G14" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="116"/>
-      <c r="I14" s="116"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
       <c r="J14" s="14">
         <f t="shared" si="0"/>
-        <v>44.728888888888889</v>
+        <v>14.8</v>
       </c>
       <c r="K14" s="15">
         <f>dadoshistoricos!F31*0.8</f>
@@ -2707,18 +2720,18 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="117"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
       <c r="F15"/>
-      <c r="G15" s="116" t="s">
+      <c r="G15" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
-        <v>11.182222222222222</v>
+        <v>3.7</v>
       </c>
       <c r="K15" s="16">
         <f>dadoshistoricos!F31*0.2</f>
@@ -2728,19 +2741,19 @@
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="111"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="116" t="s">
+      <c r="G16" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
-        <v>18.133333333333333</v>
+        <v>6</v>
       </c>
       <c r="K16" s="16">
         <f>dadoshistoricos!G31</f>
@@ -2755,14 +2768,14 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="119" t="s">
+      <c r="G17" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="119"/>
-      <c r="I17" s="119"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
       <c r="J17" s="14">
         <f t="shared" si="0"/>
-        <v>151.11111111111111</v>
+        <v>50</v>
       </c>
       <c r="K17" s="16">
         <f>dadoshistoricos!H31</f>
@@ -2777,14 +2790,14 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="119" t="s">
+      <c r="G18" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="119"/>
-      <c r="I18" s="119"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="107"/>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
-        <v>6.0444444444444443</v>
+        <v>2</v>
       </c>
       <c r="K18" s="16">
         <f>dadoshistoricos!I31</f>
@@ -2798,14 +2811,14 @@
       <c r="D19"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="119" t="s">
+      <c r="G19" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="119"/>
-      <c r="I19" s="119"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="107"/>
       <c r="J19" s="14">
         <f t="shared" si="0"/>
-        <v>18.435555555555556</v>
+        <v>6.1000000000000005</v>
       </c>
       <c r="K19" s="16">
         <f>dadoshistoricos!J31</f>
@@ -2819,14 +2832,14 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="119" t="s">
+      <c r="G20" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="119"/>
-      <c r="I20" s="119"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="107"/>
       <c r="J20" s="14">
         <f t="shared" si="0"/>
-        <v>9.6711111111111112</v>
+        <v>3.2</v>
       </c>
       <c r="K20" s="16">
         <f>dadoshistoricos!K31</f>
@@ -2840,14 +2853,14 @@
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="120" t="s">
+      <c r="G21" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
       <c r="J21" s="18">
         <f>SUM(J13:J19)</f>
-        <v>262.32888888888891</v>
+        <v>86.8</v>
       </c>
       <c r="K21" s="19">
         <f>SUM(K13:K20)</f>
@@ -2856,27 +2869,27 @@
       <c r="L21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="121"/>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
-      <c r="E22" s="121"/>
-      <c r="F22" s="121"/>
-      <c r="G22" s="121"/>
-      <c r="H22" s="121"/>
-      <c r="I22" s="121"/>
-      <c r="J22" s="121"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
       <c r="L22" s="12"/>
     </row>
     <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="122"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
-      <c r="E23" s="122"/>
-      <c r="F23" s="122"/>
-      <c r="G23" s="122"/>
-      <c r="H23" s="122"/>
-      <c r="I23" s="122"/>
-      <c r="J23" s="122"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="110"/>
       <c r="L23" s="12"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
@@ -2925,45 +2938,45 @@
       <c r="L27" s="12"/>
     </row>
     <row r="28" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="122"/>
-      <c r="C28" s="122"/>
-      <c r="D28" s="122"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="122"/>
-      <c r="I28" s="122"/>
-      <c r="J28" s="122"/>
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
     </row>
     <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:I12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2978,7 +2991,7 @@
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3009,11 +3022,11 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
       <c r="E2" s="21"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3137,7 +3150,7 @@
       </c>
       <c r="D9" s="33">
         <f>COUNTIF(Atores,B9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -3156,7 +3169,7 @@
       </c>
       <c r="D10" s="35">
         <f>(C7*D7)+(C8*D8)+(C9*D9)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -3197,7 +3210,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="37" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>25</v>
@@ -3206,7 +3219,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>25</v>
@@ -3214,8 +3227,12 @@
       <c r="F15"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="39"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>25</v>
+      </c>
       <c r="F16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -3229,7 +3246,7 @@
       </c>
       <c r="C18" s="42">
         <f>SUBTOTAL(103,C14:C17)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3256,8 +3273,8 @@
   </sheetPr>
   <dimension ref="A1:AMK1010"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3288,11 +3305,11 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
@@ -3350,7 +3367,8 @@
         <v>3</v>
       </c>
       <c r="D7" s="9">
-        <v>1</v>
+        <f>COUNTIF(CUC,B7)</f>
+        <v>18</v>
       </c>
       <c r="E7" s="51"/>
       <c r="H7"/>
@@ -3366,7 +3384,7 @@
       </c>
       <c r="D8" s="27">
         <f>COUNTIF(CUC,B8)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8" s="51"/>
       <c r="H8"/>
@@ -3382,7 +3400,7 @@
       </c>
       <c r="D9" s="27">
         <f>COUNTIF(CUC,B9)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="51"/>
       <c r="H9"/>
@@ -3396,16 +3414,16 @@
       </c>
       <c r="D10" s="57">
         <f>(C7*D7)+(C8*D8)+(C9*D9)</f>
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="E10"/>
       <c r="H10"/>
       <c r="O10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="125"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
+      <c r="A11" s="127"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="127"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="H11"/>
@@ -3433,7 +3451,7 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="62"/>
       <c r="B13" s="63" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C13" s="64">
         <v>1</v>
@@ -3451,13 +3469,13 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="62"/>
       <c r="B14" s="63" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C14" s="64">
         <v>1</v>
       </c>
       <c r="D14" s="65" t="str">
-        <f t="shared" ref="D14:D31" si="0">IF(C14&lt;4,"Simples",(IF(C14&gt;5,"Complexo","Médio")))</f>
+        <f t="shared" ref="D14:D32" si="0">IF(C14&lt;4,"Simples",(IF(C14&gt;5,"Complexo","Médio")))</f>
         <v>Simples</v>
       </c>
       <c r="E14" s="63"/>
@@ -3469,7 +3487,7 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="62"/>
       <c r="B15" s="63" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C15" s="64">
         <v>1</v>
@@ -3487,7 +3505,7 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="62"/>
       <c r="B16" s="63" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C16" s="64">
         <v>1</v>
@@ -3505,7 +3523,7 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="62"/>
       <c r="B17" s="63" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C17" s="64">
         <v>1</v>
@@ -3523,7 +3541,7 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="62"/>
       <c r="B18" s="63" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C18" s="64">
         <v>1</v>
@@ -3541,7 +3559,7 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="62"/>
       <c r="B19" s="63" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C19" s="64">
         <v>1</v>
@@ -3559,7 +3577,7 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="62"/>
       <c r="B20" s="63" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C20" s="64">
         <v>1</v>
@@ -3577,7 +3595,7 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="62"/>
       <c r="B21" s="63" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C21" s="64">
         <v>1</v>
@@ -3595,14 +3613,14 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="62"/>
       <c r="B22" s="63" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C22" s="64">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D22" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Complexo</v>
+        <v>Simples</v>
       </c>
       <c r="E22" s="63"/>
       <c r="H22" s="43"/>
@@ -3613,14 +3631,14 @@
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="62"/>
       <c r="B23" s="63" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C23" s="64">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D23" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Complexo</v>
+        <v>Simples</v>
       </c>
       <c r="E23" s="63"/>
       <c r="O23" s="20">
@@ -3630,10 +3648,10 @@
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="62"/>
       <c r="B24" s="63" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C24" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="65" t="str">
         <f t="shared" si="0"/>
@@ -3647,10 +3665,10 @@
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="62"/>
       <c r="B25" s="63" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C25" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="65" t="str">
         <f t="shared" si="0"/>
@@ -3664,14 +3682,14 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="62"/>
       <c r="B26" s="63" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C26" s="64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D26" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Simples</v>
+        <v>Médio</v>
       </c>
       <c r="E26" s="63"/>
       <c r="O26" s="20">
@@ -3681,14 +3699,14 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="62"/>
       <c r="B27" s="63" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C27" s="64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Simples</v>
+        <v>Médio</v>
       </c>
       <c r="E27" s="63"/>
       <c r="O27" s="20">
@@ -3698,14 +3716,14 @@
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="62"/>
       <c r="B28" s="63" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C28" s="64">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D28" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Complexo</v>
+        <v>Simples</v>
       </c>
       <c r="E28" s="63"/>
       <c r="O28" s="20">
@@ -3715,10 +3733,10 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="62"/>
       <c r="B29" s="63" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C29" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="65" t="str">
         <f t="shared" si="0"/>
@@ -3732,14 +3750,14 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="62"/>
       <c r="B30" s="63" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C30" s="64">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D30" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Complexo</v>
+        <v>Simples</v>
       </c>
       <c r="E30" s="63"/>
       <c r="O30" s="20">
@@ -3749,14 +3767,14 @@
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="62"/>
       <c r="B31" s="63" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C31" s="64">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D31" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Complexo</v>
+        <v>Simples</v>
       </c>
       <c r="E31" s="63"/>
       <c r="O31" s="20">
@@ -3765,9 +3783,15 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="62"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
+      <c r="B32" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="64">
+        <v>6</v>
+      </c>
+      <c r="D32" s="65" t="s">
+        <v>25</v>
+      </c>
       <c r="E32" s="63"/>
       <c r="O32" s="20">
         <v>21</v>
@@ -3775,9 +3799,15 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="62"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="65"/>
+      <c r="B33" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="64">
+        <v>1</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>23</v>
+      </c>
       <c r="E33" s="63"/>
       <c r="O33" s="20">
         <v>22</v>
@@ -3785,9 +3815,15 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="62"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65"/>
+      <c r="B34" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="64">
+        <v>4</v>
+      </c>
+      <c r="D34" s="65" t="s">
+        <v>24</v>
+      </c>
       <c r="E34" s="63"/>
       <c r="O34" s="20">
         <v>23</v>
@@ -3795,9 +3831,15 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="62"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="65"/>
+      <c r="B35" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="64">
+        <v>4</v>
+      </c>
+      <c r="D35" s="65" t="s">
+        <v>24</v>
+      </c>
       <c r="E35" s="63"/>
       <c r="O35" s="20">
         <v>24</v>
@@ -3816,7 +3858,7 @@
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="62"/>
       <c r="B37" s="63"/>
-      <c r="C37" s="133"/>
+      <c r="C37" s="105"/>
       <c r="D37" s="39"/>
       <c r="E37" s="63"/>
       <c r="O37" s="20">
@@ -3826,7 +3868,7 @@
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="62"/>
       <c r="B38" s="63"/>
-      <c r="C38" s="133"/>
+      <c r="C38" s="105"/>
       <c r="D38" s="39"/>
       <c r="E38" s="63"/>
       <c r="O38" s="20">
@@ -3836,7 +3878,7 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="62"/>
       <c r="B39" s="63"/>
-      <c r="C39" s="133"/>
+      <c r="C39" s="105"/>
       <c r="D39" s="39"/>
       <c r="E39" s="63"/>
       <c r="O39" s="20">
@@ -3849,11 +3891,11 @@
       </c>
       <c r="B40" s="66">
         <f>SUBTOTAL(103,B13:B39)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C40" s="67"/>
       <c r="D40" s="43"/>
-      <c r="E40" s="134"/>
+      <c r="E40" s="106"/>
       <c r="O40" s="20">
         <v>29</v>
       </c>
@@ -8746,7 +8788,7 @@
   </sheetPr>
   <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -8804,12 +8846,12 @@
       <c r="M3"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -8848,12 +8890,12 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="12"/>
@@ -9172,11 +9214,11 @@
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="127" t="s">
+      <c r="B22" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="127"/>
-      <c r="D22" s="127"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
       <c r="E22" s="72">
         <f>0.6+(0.01*SUM(D9*E9,D10*E10,D11*E11,D12*E12,D13*E13,D14*E14,D15*E15,D16*E16,D17*E17,D18*E18,D19*E19,D20*E20,D21*E21))</f>
         <v>0.78499999999999992</v>
@@ -9223,12 +9265,12 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="128" t="s">
+      <c r="B26" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
+      <c r="C26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="73"/>
       <c r="G26" s="74"/>
       <c r="I26"/>
@@ -9237,11 +9279,11 @@
       <c r="B27" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="129" t="s">
+      <c r="C27" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="129"/>
-      <c r="E27" s="129"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
       <c r="F27" s="75" t="s">
         <v>21</v>
       </c>
@@ -9254,11 +9296,11 @@
       <c r="B28" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="130" t="s">
+      <c r="C28" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="130"/>
-      <c r="E28" s="130"/>
+      <c r="D28" s="128"/>
+      <c r="E28" s="128"/>
       <c r="F28" s="29">
         <v>1.5</v>
       </c>
@@ -9271,11 +9313,11 @@
       <c r="B29" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="130" t="s">
+      <c r="C29" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="130"/>
-      <c r="E29" s="130"/>
+      <c r="D29" s="128"/>
+      <c r="E29" s="128"/>
       <c r="F29" s="29">
         <v>0.5</v>
       </c>
@@ -9288,11 +9330,11 @@
       <c r="B30" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="130"/>
-      <c r="E30" s="130"/>
+      <c r="D30" s="128"/>
+      <c r="E30" s="128"/>
       <c r="F30" s="29">
         <v>1</v>
       </c>
@@ -9305,11 +9347,11 @@
       <c r="B31" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="130" t="s">
+      <c r="C31" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="130"/>
-      <c r="E31" s="130"/>
+      <c r="D31" s="128"/>
+      <c r="E31" s="128"/>
       <c r="F31" s="29">
         <v>0.5</v>
       </c>
@@ -9322,11 +9364,11 @@
       <c r="B32" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="130" t="s">
+      <c r="C32" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="130"/>
-      <c r="E32" s="130"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
       <c r="F32" s="29">
         <v>1</v>
       </c>
@@ -9339,11 +9381,11 @@
       <c r="B33" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="130" t="s">
+      <c r="C33" s="128" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="130"/>
-      <c r="E33" s="130"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
       <c r="F33" s="29">
         <v>2</v>
       </c>
@@ -9356,11 +9398,11 @@
       <c r="B34" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="130" t="s">
+      <c r="C34" s="128" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="130"/>
-      <c r="E34" s="130"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
       <c r="F34" s="29">
         <v>-1</v>
       </c>
@@ -9373,11 +9415,11 @@
       <c r="B35" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="130" t="s">
+      <c r="C35" s="128" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="130"/>
-      <c r="E35" s="130"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128"/>
       <c r="F35" s="29">
         <v>-1</v>
       </c>
@@ -9387,13 +9429,13 @@
       <c r="I35" s="71"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="127" t="s">
+      <c r="B36" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="127"/>
-      <c r="D36" s="127"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
+      <c r="C36" s="129"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="129"/>
       <c r="G36" s="76">
         <f>1.4+(-0.03*SUM(F28*G28,F29*G29,F30*G30,F31*G31,F32*G32,F33*G33,F34*G34,F35*G35))</f>
         <v>0.95</v>
@@ -9403,6 +9445,11 @@
   </sheetData>
   <sheetProtection password="C6D5" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -9412,11 +9459,6 @@
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -9457,19 +9499,19 @@
   <sheetData>
     <row r="1" spans="1:55" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="77"/>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
       <c r="M1" s="78"/>
       <c r="N1" s="77"/>
       <c r="O1" s="77"/>
@@ -11264,10 +11306,10 @@
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="77"/>
-      <c r="J30" s="132" t="s">
+      <c r="J30" s="134" t="s">
         <v>102</v>
       </c>
-      <c r="K30" s="132"/>
+      <c r="K30" s="134"/>
       <c r="L30" s="99">
         <v>8</v>
       </c>

</xml_diff>